<commit_message>
Fléau de la corruption
</commit_message>
<xml_diff>
--- a/WIP/.Repartition.xlsx
+++ b/WIP/.Repartition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etien\Desktop\MtG\Proxys\HoF_EDH\WIP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E3C553-E13B-465F-B446-63EB2B5C2C6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF3C72A7-010F-44C0-BA5F-CBC00B853945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="77">
   <si>
     <t>Type</t>
   </si>
@@ -253,6 +253,9 @@
   </si>
   <si>
     <t>Iga, divinité tourmentée</t>
+  </si>
+  <si>
+    <t>Fléau de la corruption</t>
   </si>
 </sst>
 </file>
@@ -682,7 +685,7 @@
                   <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>20</c:v>
@@ -691,7 +694,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>57</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -930,16 +933,16 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>12</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1224,7 +1227,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>85</c:v>
+                  <c:v>84</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>6</c:v>
@@ -1239,7 +1242,7 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -1555,7 +1558,7 @@
                   <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>10</c:v>
@@ -4352,7 +4355,7 @@
   <dimension ref="A1:U201"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4791,7 +4794,7 @@
         <v>2</v>
       </c>
       <c r="J16" t="s">
-        <v>37</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.3">
@@ -5067,14 +5070,14 @@
         <v>3</v>
       </c>
       <c r="J25" t="s">
-        <v>37</v>
+        <v>73</v>
       </c>
       <c r="T25" t="s">
         <v>29</v>
       </c>
       <c r="U25">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.3">
@@ -5096,7 +5099,7 @@
         <v>1</v>
       </c>
       <c r="J26" t="s">
-        <v>37</v>
+        <v>73</v>
       </c>
       <c r="K26" t="s">
         <v>29</v>
@@ -5106,7 +5109,7 @@
       </c>
       <c r="U26">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.3">
@@ -5169,7 +5172,7 @@
       </c>
       <c r="U28">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.3">
@@ -5326,7 +5329,7 @@
       </c>
       <c r="U33">
         <f>COUNTIF(I:I,T33)</f>
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.3">
@@ -5484,7 +5487,7 @@
       </c>
       <c r="U38">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.3">
@@ -5772,15 +5775,29 @@
         <v>27</v>
       </c>
     </row>
-    <row r="49" spans="3:21" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>76</v>
+      </c>
+      <c r="B49" t="s">
+        <v>14</v>
+      </c>
       <c r="C49" s="2"/>
       <c r="D49" s="3"/>
-      <c r="E49" s="4"/>
+      <c r="E49" s="4">
+        <v>2</v>
+      </c>
       <c r="F49" s="5"/>
       <c r="G49" s="6"/>
+      <c r="H49">
+        <v>3</v>
+      </c>
       <c r="I49">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="J49" t="s">
+        <v>29</v>
       </c>
       <c r="T49" t="s">
         <v>8</v>
@@ -5790,7 +5807,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="50" spans="3:21" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C50" s="2"/>
       <c r="D50" s="3"/>
       <c r="E50" s="4"/>
@@ -5805,10 +5822,10 @@
       </c>
       <c r="U50">
         <f t="shared" ref="U50:U55" si="3">COUNTIF(B:B,T50)</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="51" spans="3:21" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C51" s="2"/>
       <c r="D51" s="3"/>
       <c r="E51" s="4"/>
@@ -5826,7 +5843,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="3:21" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C52" s="2"/>
       <c r="D52" s="3"/>
       <c r="E52" s="4"/>
@@ -5844,7 +5861,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="3:21" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C53" s="2"/>
       <c r="D53" s="3"/>
       <c r="E53" s="4"/>
@@ -5862,7 +5879,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="3:21" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C54" s="2"/>
       <c r="D54" s="3"/>
       <c r="E54" s="4"/>
@@ -5880,7 +5897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="3:21" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C55" s="2"/>
       <c r="D55" s="3"/>
       <c r="E55" s="4"/>
@@ -5898,7 +5915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="3:21" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C56" s="2"/>
       <c r="D56" s="3"/>
       <c r="E56" s="4"/>
@@ -5909,7 +5926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="3:21" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C57" s="2"/>
       <c r="D57" s="3"/>
       <c r="E57" s="4"/>
@@ -5920,7 +5937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="3:21" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C58" s="2"/>
       <c r="D58" s="3"/>
       <c r="E58" s="4"/>
@@ -5931,7 +5948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="3:21" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C59" s="2"/>
       <c r="D59" s="3"/>
       <c r="E59" s="4"/>
@@ -5942,7 +5959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="3:21" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C60" s="2"/>
       <c r="D60" s="3"/>
       <c r="E60" s="4"/>
@@ -5953,7 +5970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="3:21" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C61" s="2"/>
       <c r="D61" s="3"/>
       <c r="E61" s="4"/>
@@ -5964,7 +5981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="3:21" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C62" s="2"/>
       <c r="D62" s="3"/>
       <c r="E62" s="4"/>
@@ -5975,7 +5992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="3:21" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C63" s="2"/>
       <c r="D63" s="3"/>
       <c r="E63" s="4"/>
@@ -5986,7 +6003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="3:21" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C64" s="2"/>
       <c r="D64" s="3"/>
       <c r="E64" s="4"/>
@@ -6415,7 +6432,7 @@
       </c>
       <c r="E102" s="4">
         <f t="shared" si="5"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F102" s="5">
         <f t="shared" si="5"/>
@@ -6427,11 +6444,11 @@
       </c>
       <c r="H102">
         <f t="shared" si="5"/>
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="I102">
         <f>SUM(I2:I101)/(100-U52)</f>
-        <v>1.2525252525252526</v>
+        <v>1.303030303030303</v>
       </c>
     </row>
     <row r="103" spans="3:9" x14ac:dyDescent="0.3">
@@ -6854,7 +6871,7 @@
       <c r="F162" s="5"/>
       <c r="G162" s="6"/>
       <c r="I162">
-        <f t="shared" ref="I106:I169" si="6">SUM(C162:H162)</f>
+        <f t="shared" ref="I162:I169" si="6">SUM(C162:H162)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Cartes -> Anneau de vérité
</commit_message>
<xml_diff>
--- a/WIP/.Repartition.xlsx
+++ b/WIP/.Repartition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etien\Desktop\MtG\Proxys\HoF_EDH\WIP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E89C577-5529-4B4D-A04D-A6D6FE42602D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7960F3E6-B3F1-4750-A113-E61EEE688EE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="91">
   <si>
     <t>Type</t>
   </si>
@@ -271,6 +271,33 @@
   </si>
   <si>
     <t>Marchand Prospère</t>
+  </si>
+  <si>
+    <t>Maître de son destin</t>
+  </si>
+  <si>
+    <t>Espoir éternel</t>
+  </si>
+  <si>
+    <t>Triche</t>
+  </si>
+  <si>
+    <t>Capuche de parieur</t>
+  </si>
+  <si>
+    <t>Joyau du parieur</t>
+  </si>
+  <si>
+    <t>Anneau de Kallas</t>
+  </si>
+  <si>
+    <t>Anneau de concentration</t>
+  </si>
+  <si>
+    <t>Anneau de sacrifice</t>
+  </si>
+  <si>
+    <t>Anneau de vérité</t>
   </si>
 </sst>
 </file>
@@ -694,22 +721,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>16</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>21</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>70</c:v>
+                  <c:v>85</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -875,9 +902,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Feuil1!$T$17:$T$28</c:f>
+              <c:f>Feuil1!$T$17:$T$29</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>Pioche</c:v>
                 </c:pt>
@@ -914,20 +941,23 @@
                 <c:pt idx="11">
                   <c:v>Pump</c:v>
                 </c:pt>
+                <c:pt idx="12">
+                  <c:v>Triche</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$U$17:$U$28</c:f>
+              <c:f>Feuil1!$U$17:$U$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1</c:v>
@@ -958,6 +988,9 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1242,19 +1275,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>79</c:v>
+                  <c:v>71</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>19</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>4</c:v>
@@ -1582,10 +1615,10 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -4369,8 +4402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U201"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K54" sqref="K54"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4451,14 +4484,30 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="3"/>
+      <c r="D3" s="3">
+        <v>1</v>
+      </c>
       <c r="E3" s="4"/>
-      <c r="F3" s="5"/>
+      <c r="F3" s="5">
+        <v>1</v>
+      </c>
       <c r="G3" s="6"/>
+      <c r="H3">
+        <v>1</v>
+      </c>
       <c r="I3">
         <f t="shared" ref="I3:I66" si="0">SUM(C3:H3)</f>
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="J3" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -4870,7 +4919,7 @@
       </c>
       <c r="U18">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.3">
@@ -5219,9 +5268,12 @@
       <c r="K29" t="s">
         <v>29</v>
       </c>
+      <c r="T29" t="s">
+        <v>84</v>
+      </c>
       <c r="U29">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.3">
@@ -5344,7 +5396,7 @@
       </c>
       <c r="U33">
         <f>COUNTIF(I:I,T33)</f>
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.3">
@@ -5408,7 +5460,7 @@
       </c>
       <c r="U35">
         <f t="shared" si="2"/>
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.3">
@@ -5439,7 +5491,7 @@
       </c>
       <c r="U36">
         <f t="shared" si="2"/>
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.3">
@@ -5471,7 +5523,7 @@
       </c>
       <c r="U37">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.3">
@@ -5948,14 +6000,14 @@
         <v>3</v>
       </c>
       <c r="J53" t="s">
-        <v>29</v>
+        <v>84</v>
       </c>
       <c r="T53" t="s">
         <v>18</v>
       </c>
       <c r="U53">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="54" spans="1:21" x14ac:dyDescent="0.3">
@@ -5987,18 +6039,34 @@
       </c>
       <c r="U54">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="C55" s="2"/>
-      <c r="D55" s="3"/>
+      <c r="A55" t="s">
+        <v>83</v>
+      </c>
+      <c r="B55" t="s">
+        <v>18</v>
+      </c>
+      <c r="C55" s="2">
+        <v>1</v>
+      </c>
+      <c r="D55" s="3">
+        <v>1</v>
+      </c>
       <c r="E55" s="4"/>
       <c r="F55" s="5"/>
       <c r="G55" s="6"/>
+      <c r="H55">
+        <v>2</v>
+      </c>
       <c r="I55">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="J55" t="s">
+        <v>84</v>
       </c>
       <c r="T55" t="s">
         <v>11</v>
@@ -6009,69 +6077,147 @@
       </c>
     </row>
     <row r="56" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>85</v>
+      </c>
+      <c r="B56" t="s">
+        <v>19</v>
+      </c>
       <c r="C56" s="2"/>
       <c r="D56" s="3"/>
       <c r="E56" s="4"/>
       <c r="F56" s="5"/>
       <c r="G56" s="6"/>
+      <c r="H56">
+        <v>2</v>
+      </c>
       <c r="I56">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="J56" t="s">
+        <v>84</v>
+      </c>
+      <c r="K56" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="57" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>86</v>
+      </c>
+      <c r="B57" t="s">
+        <v>19</v>
+      </c>
       <c r="C57" s="2"/>
       <c r="D57" s="3"/>
       <c r="E57" s="4"/>
       <c r="F57" s="5"/>
       <c r="G57" s="6"/>
+      <c r="H57">
+        <v>2</v>
+      </c>
       <c r="I57">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="J57" t="s">
+        <v>84</v>
+      </c>
+      <c r="K57" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="58" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>87</v>
+      </c>
+      <c r="B58" t="s">
+        <v>19</v>
+      </c>
       <c r="C58" s="2"/>
       <c r="D58" s="3"/>
       <c r="E58" s="4"/>
       <c r="F58" s="5"/>
       <c r="G58" s="6"/>
+      <c r="H58">
+        <v>2</v>
+      </c>
       <c r="I58">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="J58" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="59" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>88</v>
+      </c>
+      <c r="B59" t="s">
+        <v>19</v>
+      </c>
       <c r="C59" s="2"/>
       <c r="D59" s="3"/>
       <c r="E59" s="4"/>
       <c r="F59" s="5"/>
       <c r="G59" s="6"/>
+      <c r="H59">
+        <v>2</v>
+      </c>
       <c r="I59">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="J59" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="60" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>89</v>
+      </c>
+      <c r="B60" t="s">
+        <v>19</v>
+      </c>
       <c r="C60" s="2"/>
       <c r="D60" s="3"/>
       <c r="E60" s="4"/>
       <c r="F60" s="5"/>
       <c r="G60" s="6"/>
+      <c r="H60">
+        <v>2</v>
+      </c>
       <c r="I60">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="J60" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="61" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>90</v>
+      </c>
+      <c r="B61" t="s">
+        <v>19</v>
+      </c>
       <c r="C61" s="2"/>
       <c r="D61" s="3"/>
       <c r="E61" s="4"/>
       <c r="F61" s="5"/>
       <c r="G61" s="6"/>
+      <c r="H61">
+        <v>2</v>
+      </c>
       <c r="I61">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="J61" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="62" spans="1:21" x14ac:dyDescent="0.3">
@@ -6517,11 +6663,11 @@
     <row r="102" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C102" s="2">
         <f t="shared" ref="C102:H102" si="5">SUM(C2:C101)</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D102" s="3">
         <f t="shared" si="5"/>
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E102" s="4">
         <f t="shared" si="5"/>
@@ -6529,7 +6675,7 @@
       </c>
       <c r="F102" s="5">
         <f t="shared" si="5"/>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G102" s="6">
         <f t="shared" si="5"/>
@@ -6537,11 +6683,11 @@
       </c>
       <c r="H102">
         <f t="shared" si="5"/>
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="I102">
         <f>SUM(I2:I101)/(100-U52)</f>
-        <v>1.4747474747474747</v>
+        <v>1.6666666666666667</v>
       </c>
     </row>
     <row r="103" spans="3:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Terrains -> Croisée des chemins + Basics
</commit_message>
<xml_diff>
--- a/WIP/.Repartition.xlsx
+++ b/WIP/.Repartition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etien\Desktop\MtG\Proxys\HoF_EDH\WIP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7960F3E6-B3F1-4750-A113-E61EEE688EE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{033D2328-38AD-4FA5-9851-FFFF763085AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="104">
   <si>
     <t>Type</t>
   </si>
@@ -298,6 +298,45 @@
   </si>
   <si>
     <t>Anneau de vérité</t>
+  </si>
+  <si>
+    <t>Appel de la victoire</t>
+  </si>
+  <si>
+    <t>Gantelet d'occultiste</t>
+  </si>
+  <si>
+    <t>Carreau foudroyant</t>
+  </si>
+  <si>
+    <t>Armure d'écailles du roi mort</t>
+  </si>
+  <si>
+    <t>Grobben, chef de la Fosse</t>
+  </si>
+  <si>
+    <t>La Vieille Dame</t>
+  </si>
+  <si>
+    <t>Ruines de la Tour</t>
+  </si>
+  <si>
+    <t>Frontière de la province</t>
+  </si>
+  <si>
+    <t>Campement sauvage</t>
+  </si>
+  <si>
+    <t>Campement sous les étoiles</t>
+  </si>
+  <si>
+    <t>Campement souterrain</t>
+  </si>
+  <si>
+    <t>Campement urbain</t>
+  </si>
+  <si>
+    <t>Croisée des chemins</t>
   </si>
 </sst>
 </file>
@@ -721,7 +760,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>17</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>20</c:v>
@@ -730,13 +769,13 @@
                   <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>22</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>85</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -957,13 +996,13 @@
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>12</c:v>
@@ -975,10 +1014,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>17</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>7</c:v>
@@ -987,7 +1026,7 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>5</c:v>
@@ -1275,13 +1314,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>71</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>20</c:v>
@@ -1293,7 +1332,7 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>1</c:v>
@@ -1603,7 +1642,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>22</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>8</c:v>
@@ -1612,13 +1651,13 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -4402,8 +4441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4919,7 +4958,7 @@
       </c>
       <c r="U18">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.3">
@@ -4943,7 +4982,7 @@
       </c>
       <c r="U19">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.3">
@@ -4975,7 +5014,7 @@
       </c>
       <c r="U20">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.3">
@@ -5109,7 +5148,7 @@
       </c>
       <c r="U24">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.3">
@@ -5141,7 +5180,7 @@
       </c>
       <c r="U25">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.3">
@@ -5236,7 +5275,7 @@
       </c>
       <c r="U28">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.3">
@@ -5396,7 +5435,7 @@
       </c>
       <c r="U33">
         <f>COUNTIF(I:I,T33)</f>
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.3">
@@ -5428,7 +5467,7 @@
       </c>
       <c r="U34">
         <f t="shared" ref="U34:U42" si="2">COUNTIF(I:I,T34)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.3">
@@ -5460,7 +5499,7 @@
       </c>
       <c r="U35">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.3">
@@ -5586,7 +5625,7 @@
       </c>
       <c r="U39">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.3">
@@ -5857,11 +5896,11 @@
       <c r="F49" s="5"/>
       <c r="G49" s="6"/>
       <c r="H49">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I49">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J49" t="s">
         <v>29</v>
@@ -5871,7 +5910,7 @@
       </c>
       <c r="U49">
         <f>COUNTIF(B:B,T49)</f>
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.3">
@@ -5975,7 +6014,7 @@
       </c>
       <c r="U52">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>35</v>
       </c>
     </row>
     <row r="53" spans="1:21" x14ac:dyDescent="0.3">
@@ -6039,7 +6078,7 @@
       </c>
       <c r="U54">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.3">
@@ -6221,107 +6260,238 @@
       </c>
     </row>
     <row r="62" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>91</v>
+      </c>
+      <c r="B62" t="s">
+        <v>19</v>
+      </c>
       <c r="C62" s="2"/>
       <c r="D62" s="3"/>
       <c r="E62" s="4"/>
       <c r="F62" s="5"/>
       <c r="G62" s="6"/>
+      <c r="H62">
+        <v>1</v>
+      </c>
       <c r="I62">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="J62" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="63" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>92</v>
+      </c>
+      <c r="B63" t="s">
+        <v>19</v>
+      </c>
       <c r="C63" s="2"/>
       <c r="D63" s="3"/>
       <c r="E63" s="4"/>
       <c r="F63" s="5"/>
       <c r="G63" s="6"/>
+      <c r="H63">
+        <v>2</v>
+      </c>
       <c r="I63">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="J63" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="64" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>93</v>
+      </c>
+      <c r="B64" t="s">
+        <v>19</v>
+      </c>
       <c r="C64" s="2"/>
       <c r="D64" s="3"/>
       <c r="E64" s="4"/>
       <c r="F64" s="5"/>
       <c r="G64" s="6"/>
+      <c r="H64">
+        <v>1</v>
+      </c>
       <c r="I64">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="3:9" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="J64" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>94</v>
+      </c>
+      <c r="B65" t="s">
+        <v>19</v>
+      </c>
       <c r="C65" s="2"/>
       <c r="D65" s="3"/>
       <c r="E65" s="4"/>
       <c r="F65" s="5"/>
       <c r="G65" s="6"/>
+      <c r="H65">
+        <v>2</v>
+      </c>
       <c r="I65">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="3:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="J65" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>95</v>
+      </c>
+      <c r="B66" t="s">
+        <v>8</v>
+      </c>
       <c r="C66" s="2"/>
       <c r="D66" s="3"/>
       <c r="E66" s="4"/>
-      <c r="F66" s="5"/>
+      <c r="F66" s="5">
+        <v>2</v>
+      </c>
       <c r="G66" s="6"/>
+      <c r="H66">
+        <v>3</v>
+      </c>
       <c r="I66">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C67" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="J66" t="s">
+        <v>29</v>
+      </c>
+      <c r="K66" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>96</v>
+      </c>
+      <c r="B67" t="s">
+        <v>8</v>
+      </c>
+      <c r="C67" s="2">
+        <v>1</v>
+      </c>
       <c r="D67" s="3"/>
       <c r="E67" s="4"/>
       <c r="F67" s="5"/>
       <c r="G67" s="6"/>
+      <c r="H67">
+        <v>1</v>
+      </c>
       <c r="I67">
         <f t="shared" ref="I67:I101" si="4">SUM(C67:H67)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C68" s="2"/>
-      <c r="D68" s="3"/>
-      <c r="E68" s="4"/>
-      <c r="F68" s="5"/>
+        <v>2</v>
+      </c>
+      <c r="J67" t="s">
+        <v>29</v>
+      </c>
+      <c r="K67" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>97</v>
+      </c>
+      <c r="B68" t="s">
+        <v>17</v>
+      </c>
+      <c r="C68" s="2">
+        <v>0</v>
+      </c>
+      <c r="D68" s="3">
+        <v>0</v>
+      </c>
+      <c r="E68" s="4">
+        <v>0</v>
+      </c>
+      <c r="F68" s="5">
+        <v>0</v>
+      </c>
       <c r="G68" s="6"/>
       <c r="I68">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C69" s="2"/>
-      <c r="D69" s="3"/>
-      <c r="E69" s="4"/>
-      <c r="F69" s="5"/>
-      <c r="G69" s="6"/>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>98</v>
+      </c>
+      <c r="B69" t="s">
+        <v>17</v>
+      </c>
+      <c r="C69" s="2">
+        <v>0</v>
+      </c>
+      <c r="D69" s="3">
+        <v>0</v>
+      </c>
+      <c r="E69" s="4">
+        <v>0</v>
+      </c>
+      <c r="F69" s="5">
+        <v>0</v>
+      </c>
+      <c r="G69" s="6">
+        <v>0</v>
+      </c>
       <c r="I69">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>99</v>
+      </c>
+      <c r="B70" t="s">
+        <v>17</v>
+      </c>
       <c r="C70" s="2"/>
       <c r="D70" s="3"/>
       <c r="E70" s="4"/>
-      <c r="F70" s="5"/>
+      <c r="F70" s="5">
+        <v>0</v>
+      </c>
       <c r="G70" s="6"/>
       <c r="I70">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="J70" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>100</v>
+      </c>
+      <c r="B71" t="s">
+        <v>17</v>
+      </c>
       <c r="C71" s="2"/>
-      <c r="D71" s="3"/>
+      <c r="D71" s="3">
+        <v>0</v>
+      </c>
       <c r="E71" s="4"/>
       <c r="F71" s="5"/>
       <c r="G71" s="6"/>
@@ -6329,20 +6499,48 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="J71" t="s">
+        <v>29</v>
+      </c>
+      <c r="K71" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>101</v>
+      </c>
+      <c r="B72" t="s">
+        <v>17</v>
+      </c>
       <c r="C72" s="2"/>
       <c r="D72" s="3"/>
-      <c r="E72" s="4"/>
+      <c r="E72" s="4">
+        <v>0</v>
+      </c>
       <c r="F72" s="5"/>
       <c r="G72" s="6"/>
       <c r="I72">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C73" s="2"/>
+      <c r="J72" t="s">
+        <v>29</v>
+      </c>
+      <c r="K72" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>102</v>
+      </c>
+      <c r="B73" t="s">
+        <v>17</v>
+      </c>
+      <c r="C73" s="2">
+        <v>0</v>
+      </c>
       <c r="D73" s="3"/>
       <c r="E73" s="4"/>
       <c r="F73" s="5"/>
@@ -6351,19 +6549,45 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C74" s="2"/>
-      <c r="D74" s="3"/>
-      <c r="E74" s="4"/>
-      <c r="F74" s="5"/>
+      <c r="J73" t="s">
+        <v>29</v>
+      </c>
+      <c r="K73" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>103</v>
+      </c>
+      <c r="B74" t="s">
+        <v>17</v>
+      </c>
+      <c r="C74" s="2">
+        <v>0</v>
+      </c>
+      <c r="D74" s="3">
+        <v>0</v>
+      </c>
+      <c r="E74" s="4">
+        <v>0</v>
+      </c>
+      <c r="F74" s="5">
+        <v>0</v>
+      </c>
       <c r="G74" s="6"/>
       <c r="I74">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="J74" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B75" t="s">
+        <v>17</v>
+      </c>
       <c r="C75" s="2"/>
       <c r="D75" s="3"/>
       <c r="E75" s="4"/>
@@ -6374,7 +6598,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B76" t="s">
+        <v>17</v>
+      </c>
       <c r="C76" s="2"/>
       <c r="D76" s="3"/>
       <c r="E76" s="4"/>
@@ -6385,7 +6612,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B77" t="s">
+        <v>17</v>
+      </c>
       <c r="C77" s="2"/>
       <c r="D77" s="3"/>
       <c r="E77" s="4"/>
@@ -6396,7 +6626,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B78" t="s">
+        <v>17</v>
+      </c>
       <c r="C78" s="2"/>
       <c r="D78" s="3"/>
       <c r="E78" s="4"/>
@@ -6407,7 +6640,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B79" t="s">
+        <v>17</v>
+      </c>
       <c r="C79" s="2"/>
       <c r="D79" s="3"/>
       <c r="E79" s="4"/>
@@ -6418,7 +6654,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B80" t="s">
+        <v>17</v>
+      </c>
       <c r="C80" s="2"/>
       <c r="D80" s="3"/>
       <c r="E80" s="4"/>
@@ -6429,7 +6668,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B81" t="s">
+        <v>17</v>
+      </c>
       <c r="C81" s="2"/>
       <c r="D81" s="3"/>
       <c r="E81" s="4"/>
@@ -6440,7 +6682,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B82" t="s">
+        <v>17</v>
+      </c>
       <c r="C82" s="2"/>
       <c r="D82" s="3"/>
       <c r="E82" s="4"/>
@@ -6451,7 +6696,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B83" t="s">
+        <v>17</v>
+      </c>
       <c r="C83" s="2"/>
       <c r="D83" s="3"/>
       <c r="E83" s="4"/>
@@ -6462,7 +6710,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B84" t="s">
+        <v>17</v>
+      </c>
       <c r="C84" s="2"/>
       <c r="D84" s="3"/>
       <c r="E84" s="4"/>
@@ -6473,7 +6724,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B85" t="s">
+        <v>17</v>
+      </c>
       <c r="C85" s="2"/>
       <c r="D85" s="3"/>
       <c r="E85" s="4"/>
@@ -6484,7 +6738,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B86" t="s">
+        <v>17</v>
+      </c>
       <c r="C86" s="2"/>
       <c r="D86" s="3"/>
       <c r="E86" s="4"/>
@@ -6495,7 +6752,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B87" t="s">
+        <v>17</v>
+      </c>
       <c r="C87" s="2"/>
       <c r="D87" s="3"/>
       <c r="E87" s="4"/>
@@ -6506,7 +6766,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B88" t="s">
+        <v>17</v>
+      </c>
       <c r="C88" s="2"/>
       <c r="D88" s="3"/>
       <c r="E88" s="4"/>
@@ -6517,7 +6780,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B89" t="s">
+        <v>17</v>
+      </c>
       <c r="C89" s="2"/>
       <c r="D89" s="3"/>
       <c r="E89" s="4"/>
@@ -6528,7 +6794,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B90" t="s">
+        <v>17</v>
+      </c>
       <c r="C90" s="2"/>
       <c r="D90" s="3"/>
       <c r="E90" s="4"/>
@@ -6539,7 +6808,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B91" t="s">
+        <v>17</v>
+      </c>
       <c r="C91" s="2"/>
       <c r="D91" s="3"/>
       <c r="E91" s="4"/>
@@ -6550,7 +6822,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B92" t="s">
+        <v>17</v>
+      </c>
       <c r="C92" s="2"/>
       <c r="D92" s="3"/>
       <c r="E92" s="4"/>
@@ -6561,7 +6836,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B93" t="s">
+        <v>17</v>
+      </c>
       <c r="C93" s="2"/>
       <c r="D93" s="3"/>
       <c r="E93" s="4"/>
@@ -6572,7 +6850,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B94" t="s">
+        <v>17</v>
+      </c>
       <c r="C94" s="2"/>
       <c r="D94" s="3"/>
       <c r="E94" s="4"/>
@@ -6583,7 +6864,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B95" t="s">
+        <v>17</v>
+      </c>
       <c r="C95" s="2"/>
       <c r="D95" s="3"/>
       <c r="E95" s="4"/>
@@ -6594,7 +6878,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B96" t="s">
+        <v>17</v>
+      </c>
       <c r="C96" s="2"/>
       <c r="D96" s="3"/>
       <c r="E96" s="4"/>
@@ -6605,7 +6892,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B97" t="s">
+        <v>17</v>
+      </c>
       <c r="C97" s="2"/>
       <c r="D97" s="3"/>
       <c r="E97" s="4"/>
@@ -6616,7 +6906,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B98" t="s">
+        <v>17</v>
+      </c>
       <c r="C98" s="2"/>
       <c r="D98" s="3"/>
       <c r="E98" s="4"/>
@@ -6627,7 +6920,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B99" t="s">
+        <v>17</v>
+      </c>
       <c r="C99" s="2"/>
       <c r="D99" s="3"/>
       <c r="E99" s="4"/>
@@ -6638,7 +6934,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B100" t="s">
+        <v>17</v>
+      </c>
       <c r="C100" s="2"/>
       <c r="D100" s="3"/>
       <c r="E100" s="4"/>
@@ -6649,7 +6948,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B101" t="s">
+        <v>17</v>
+      </c>
       <c r="C101" s="2"/>
       <c r="D101" s="3"/>
       <c r="E101" s="4"/>
@@ -6660,10 +6962,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C102" s="2">
         <f t="shared" ref="C102:H102" si="5">SUM(C2:C101)</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D102" s="3">
         <f t="shared" si="5"/>
@@ -6675,7 +6977,7 @@
       </c>
       <c r="F102" s="5">
         <f t="shared" si="5"/>
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G102" s="6">
         <f t="shared" si="5"/>
@@ -6683,77 +6985,77 @@
       </c>
       <c r="H102">
         <f t="shared" si="5"/>
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="I102">
         <f>SUM(I2:I101)/(100-U52)</f>
-        <v>1.6666666666666667</v>
-      </c>
-    </row>
-    <row r="103" spans="3:9" x14ac:dyDescent="0.3">
+        <v>2.7538461538461538</v>
+      </c>
+    </row>
+    <row r="103" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C103" s="2"/>
       <c r="D103" s="3"/>
       <c r="E103" s="4"/>
       <c r="F103" s="5"/>
       <c r="G103" s="6"/>
     </row>
-    <row r="104" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C104" s="2"/>
       <c r="D104" s="3"/>
       <c r="E104" s="4"/>
       <c r="F104" s="5"/>
       <c r="G104" s="6"/>
     </row>
-    <row r="105" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C105" s="2"/>
       <c r="D105" s="3"/>
       <c r="E105" s="4"/>
       <c r="F105" s="5"/>
       <c r="G105" s="6"/>
     </row>
-    <row r="106" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C106" s="2"/>
       <c r="D106" s="3"/>
       <c r="E106" s="4"/>
       <c r="F106" s="5"/>
       <c r="G106" s="6"/>
     </row>
-    <row r="107" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C107" s="2"/>
       <c r="D107" s="3"/>
       <c r="E107" s="4"/>
       <c r="F107" s="5"/>
       <c r="G107" s="6"/>
     </row>
-    <row r="108" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C108" s="2"/>
       <c r="D108" s="3"/>
       <c r="E108" s="4"/>
       <c r="F108" s="5"/>
       <c r="G108" s="6"/>
     </row>
-    <row r="109" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C109" s="2"/>
       <c r="D109" s="3"/>
       <c r="E109" s="4"/>
       <c r="F109" s="5"/>
       <c r="G109" s="6"/>
     </row>
-    <row r="110" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C110" s="2"/>
       <c r="D110" s="3"/>
       <c r="E110" s="4"/>
       <c r="F110" s="5"/>
       <c r="G110" s="6"/>
     </row>
-    <row r="111" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C111" s="2"/>
       <c r="D111" s="3"/>
       <c r="E111" s="4"/>
       <c r="F111" s="5"/>
       <c r="G111" s="6"/>
     </row>
-    <row r="112" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C112" s="2"/>
       <c r="D112" s="3"/>
       <c r="E112" s="4"/>

</xml_diff>

<commit_message>
Bilands 1 à 4
</commit_message>
<xml_diff>
--- a/WIP/.Repartition.xlsx
+++ b/WIP/.Repartition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etien\Desktop\MtG\Proxys\HoF_EDH\WIP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{033D2328-38AD-4FA5-9851-FFFF763085AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB8CEE38-51FF-48AD-B37C-84E3551519A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="108">
   <si>
     <t>Type</t>
   </si>
@@ -337,6 +337,18 @@
   </si>
   <si>
     <t>Croisée des chemins</t>
+  </si>
+  <si>
+    <t>Champ des fées</t>
+  </si>
+  <si>
+    <t>Portal magique</t>
+  </si>
+  <si>
+    <t>Forteresse impériale</t>
+  </si>
+  <si>
+    <t>Egouts de la ville</t>
   </si>
 </sst>
 </file>
@@ -4441,8 +4453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75"/>
+    <sheetView tabSelected="1" topLeftCell="A60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6585,11 +6597,18 @@
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>104</v>
+      </c>
       <c r="B75" t="s">
         <v>17</v>
       </c>
-      <c r="C75" s="2"/>
-      <c r="D75" s="3"/>
+      <c r="C75" s="2">
+        <v>0</v>
+      </c>
+      <c r="D75" s="3">
+        <v>0</v>
+      </c>
       <c r="E75" s="4"/>
       <c r="F75" s="5"/>
       <c r="G75" s="6"/>
@@ -6599,13 +6618,20 @@
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>105</v>
+      </c>
       <c r="B76" t="s">
         <v>17</v>
       </c>
       <c r="C76" s="2"/>
-      <c r="D76" s="3"/>
+      <c r="D76" s="3">
+        <v>0</v>
+      </c>
       <c r="E76" s="4"/>
-      <c r="F76" s="5"/>
+      <c r="F76" s="5">
+        <v>0</v>
+      </c>
       <c r="G76" s="6"/>
       <c r="I76">
         <f t="shared" si="4"/>
@@ -6613,13 +6639,20 @@
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>106</v>
+      </c>
       <c r="B77" t="s">
         <v>17</v>
       </c>
-      <c r="C77" s="2"/>
+      <c r="C77" s="2">
+        <v>0</v>
+      </c>
       <c r="D77" s="3"/>
       <c r="E77" s="4"/>
-      <c r="F77" s="5"/>
+      <c r="F77" s="5">
+        <v>0</v>
+      </c>
       <c r="G77" s="6"/>
       <c r="I77">
         <f t="shared" si="4"/>
@@ -6627,12 +6660,19 @@
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>107</v>
+      </c>
       <c r="B78" t="s">
         <v>17</v>
       </c>
       <c r="C78" s="2"/>
-      <c r="D78" s="3"/>
-      <c r="E78" s="4"/>
+      <c r="D78" s="3">
+        <v>0</v>
+      </c>
+      <c r="E78" s="4">
+        <v>0</v>
+      </c>
       <c r="F78" s="5"/>
       <c r="G78" s="6"/>
       <c r="I78">

</xml_diff>

<commit_message>
Grimalkin + Rituel sacrificiel
</commit_message>
<xml_diff>
--- a/WIP/.Repartition.xlsx
+++ b/WIP/.Repartition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etien\Desktop\MtG\Proxys\HoF_EDH\WIP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F417E497-3FD7-488D-A397-3587BC10A5C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4603ED3A-8624-4A4B-9B0B-EB7D34F77412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="129">
   <si>
     <t>Nom</t>
   </si>
@@ -406,6 +406,12 @@
   </si>
   <si>
     <t>Marais</t>
+  </si>
+  <si>
+    <t>Grimalkin</t>
+  </si>
+  <si>
+    <t>Rituel sacrificiel</t>
   </si>
 </sst>
 </file>
@@ -782,6 +788,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="1"/>
               <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-3E2E-4D84-B705-0FDEDBEA4420}"/>
                 </c:ext>
@@ -813,6 +820,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="1"/>
               <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000003-3E2E-4D84-B705-0FDEDBEA4420}"/>
                 </c:ext>
@@ -884,6 +892,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="1"/>
               <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000007-3E2E-4D84-B705-0FDEDBEA4420}"/>
                 </c:ext>
@@ -915,6 +924,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="1"/>
               <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000009-3E2E-4D84-B705-0FDEDBEA4420}"/>
                 </c:ext>
@@ -946,6 +956,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="1"/>
               <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{0000000B-3E2E-4D84-B705-0FDEDBEA4420}"/>
                 </c:ext>
@@ -1212,10 +1223,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>11</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>3</c:v>
@@ -1245,7 +1256,7 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>5</c:v>
@@ -1531,13 +1542,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>122</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>20</c:v>
@@ -1546,7 +1557,7 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1</c:v>
@@ -2438,7 +2449,7 @@
   <dimension ref="A1:U201"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A93" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A105" sqref="A105"/>
+      <selection activeCell="K107" sqref="K107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2922,7 +2933,7 @@
       </c>
       <c r="U17">
         <f t="shared" ref="U17:U32" si="1">COUNTIF(J:J,T17)+COUNTIF(K:K,T17)</f>
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.3">
@@ -2954,7 +2965,7 @@
       </c>
       <c r="U18">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.3">
@@ -3271,7 +3282,7 @@
       </c>
       <c r="U28">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.3">
@@ -3431,7 +3442,7 @@
       </c>
       <c r="U33">
         <f t="shared" ref="U33:U42" si="2">COUNTIF(I:I,T33)</f>
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.3">
@@ -3495,7 +3506,7 @@
       </c>
       <c r="U35">
         <f t="shared" si="2"/>
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.3">
@@ -3589,7 +3600,7 @@
       </c>
       <c r="U38">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.3">
@@ -5026,7 +5037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>124</v>
       </c>
@@ -5043,7 +5054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>125</v>
       </c>
@@ -5056,11 +5067,11 @@
       <c r="F98" s="5"/>
       <c r="G98" s="6"/>
       <c r="I98">
-        <f t="shared" ref="I98:I129" si="6">SUM(C98:H98)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+        <f t="shared" ref="I98:I101" si="6">SUM(C98:H98)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>125</v>
       </c>
@@ -5077,7 +5088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>126</v>
       </c>
@@ -5094,7 +5105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>126</v>
       </c>
@@ -5111,7 +5122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C102" s="2">
         <f t="shared" ref="C102:H102" si="7">SUM(C2:C101)</f>
         <v>18</v>
@@ -5141,43 +5152,70 @@
         <v>2.7538461538461538</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C103" s="2"/>
       <c r="D103" s="3"/>
       <c r="E103" s="4"/>
       <c r="F103" s="5"/>
       <c r="G103" s="6"/>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C104" s="2"/>
       <c r="D104" s="3"/>
       <c r="E104" s="4"/>
       <c r="F104" s="5"/>
       <c r="G104" s="6"/>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C105" s="2"/>
-      <c r="D105" s="3"/>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>127</v>
+      </c>
+      <c r="C105" s="2">
+        <v>1</v>
+      </c>
+      <c r="D105" s="3">
+        <v>1</v>
+      </c>
       <c r="E105" s="4"/>
       <c r="F105" s="5"/>
       <c r="G105" s="6"/>
       <c r="I105">
         <f>SUM(C105:H105)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="J105" t="s">
+        <v>39</v>
+      </c>
+      <c r="K105" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>128</v>
+      </c>
       <c r="C106" s="2"/>
       <c r="D106" s="3"/>
-      <c r="E106" s="4"/>
+      <c r="E106" s="4">
+        <v>3</v>
+      </c>
       <c r="F106" s="5"/>
       <c r="G106" s="6"/>
+      <c r="H106">
+        <v>2</v>
+      </c>
       <c r="I106">
         <f t="shared" ref="I106:I169" si="8">SUM(C106:H106)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="J106" t="s">
+        <v>14</v>
+      </c>
+      <c r="K106" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C107" s="2"/>
       <c r="D107" s="3"/>
       <c r="E107" s="4"/>
@@ -5188,7 +5226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C108" s="2"/>
       <c r="D108" s="3"/>
       <c r="E108" s="4"/>
@@ -5199,7 +5237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C109" s="2"/>
       <c r="D109" s="3"/>
       <c r="E109" s="4"/>
@@ -5210,7 +5248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C110" s="2"/>
       <c r="D110" s="3"/>
       <c r="E110" s="4"/>
@@ -5221,7 +5259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C111" s="2"/>
       <c r="D111" s="3"/>
       <c r="E111" s="4"/>
@@ -5232,7 +5270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C112" s="2"/>
       <c r="D112" s="3"/>
       <c r="E112" s="4"/>

</xml_diff>

<commit_message>
Rituel sacrificiel renommé en Rituel d'abandon
</commit_message>
<xml_diff>
--- a/WIP/.Repartition.xlsx
+++ b/WIP/.Repartition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etien\Desktop\MtG\Proxys\HoF_EDH\WIP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4603ED3A-8624-4A4B-9B0B-EB7D34F77412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A04C421-9E95-4EBD-8C83-CD0DFCE38D7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -411,7 +411,7 @@
     <t>Grimalkin</t>
   </si>
   <si>
-    <t>Rituel sacrificiel</t>
+    <t>Rituel d'abandon</t>
   </si>
 </sst>
 </file>
@@ -2449,7 +2449,7 @@
   <dimension ref="A1:U201"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A93" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K107" sqref="K107"/>
+      <selection activeCell="A107" sqref="A107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>